<commit_message>
Resultados SETAR, ARMA yARIMA
</commit_message>
<xml_diff>
--- a/codigo_final_organizado/Simulaciones/NO_lineal_estacionario/resultados_2_ESCENARIOS_SETAR.xlsx
+++ b/codigo_final_organizado/Simulaciones/NO_lineal_estacionario/resultados_2_ESCENARIOS_SETAR.xlsx
@@ -536,19 +536,19 @@
         <v>-0.1576794063200361</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1440622979706215</v>
+        <v>0.1920478055701966</v>
       </c>
       <c r="H2" t="n">
         <v>0.3231141130128508</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2843927176435826</v>
+        <v>0.2931153080917904</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2296205259465524</v>
+        <v>0.2240828618179215</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7599649520574874</v>
+        <v>0.7639291549634947</v>
       </c>
       <c r="L2" t="n">
         <v>0.4906307953793766</v>
@@ -560,7 +560,7 @@
         <v>0.4134802190192442</v>
       </c>
       <c r="O2" t="n">
-        <v>0.2570749643498463</v>
+        <v>0.3018189596204621</v>
       </c>
     </row>
     <row r="3">
@@ -589,31 +589,31 @@
         <v>0.9771613873707746</v>
       </c>
       <c r="G3" t="n">
-        <v>1.035152805976046</v>
+        <v>0.8440802290461885</v>
       </c>
       <c r="H3" t="n">
         <v>0.8971380629950961</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9752771306597592</v>
+        <v>0.9486587492742637</v>
       </c>
       <c r="J3" t="n">
-        <v>0.8084052810575328</v>
+        <v>0.8030715638437396</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9206032848155838</v>
+        <v>0.9200936938865002</v>
       </c>
       <c r="L3" t="n">
         <v>0.963195275359668</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8271701227900183</v>
+        <v>1.344919739557854</v>
       </c>
       <c r="N3" t="n">
         <v>1.429328977467928</v>
       </c>
       <c r="O3" t="n">
-        <v>1.001415683358563</v>
+        <v>1.147772757933678</v>
       </c>
     </row>
     <row r="4">
@@ -642,31 +642,31 @@
         <v>-0.7514160756679074</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2779592771894007</v>
+        <v>0.3205563771652512</v>
       </c>
       <c r="H4" t="n">
         <v>0.3209898055826283</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2559520121250701</v>
+        <v>0.2765914636051733</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4235001238123146</v>
+        <v>0.4265827512322169</v>
       </c>
       <c r="K4" t="n">
-        <v>0.7026878665757854</v>
+        <v>0.706912652919841</v>
       </c>
       <c r="L4" t="n">
         <v>0.2439267986604944</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2970160980869537</v>
+        <v>0.2898130628153743</v>
       </c>
       <c r="N4" t="n">
         <v>0.2231246744978527</v>
       </c>
       <c r="O4" t="n">
-        <v>0.4738845108352087</v>
+        <v>0.6361204696781061</v>
       </c>
     </row>
     <row r="5">
@@ -695,31 +695,31 @@
         <v>-2.218401011803054</v>
       </c>
       <c r="G5" t="n">
-        <v>1.472810271355045</v>
+        <v>1.438599549706423</v>
       </c>
       <c r="H5" t="n">
         <v>1.604614918095754</v>
       </c>
       <c r="I5" t="n">
-        <v>1.267333129669654</v>
+        <v>1.227672168773977</v>
       </c>
       <c r="J5" t="n">
-        <v>1.46338615318703</v>
+        <v>1.902151601688216</v>
       </c>
       <c r="K5" t="n">
-        <v>0.8292438813679825</v>
+        <v>0.8355873218281257</v>
       </c>
       <c r="L5" t="n">
         <v>1.738231484259985</v>
       </c>
       <c r="M5" t="n">
-        <v>1.899999810031461</v>
+        <v>0.7818175215325235</v>
       </c>
       <c r="N5" t="n">
         <v>0.8386608194390208</v>
       </c>
       <c r="O5" t="n">
-        <v>1.387701772855472</v>
+        <v>1.164045658562616</v>
       </c>
     </row>
     <row r="6">
@@ -748,31 +748,31 @@
         <v>-1.618314180070109</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9167070556271031</v>
+        <v>0.9131169179845734</v>
       </c>
       <c r="H6" t="n">
         <v>0.6015351021412634</v>
       </c>
       <c r="I6" t="n">
-        <v>0.6473857819393163</v>
+        <v>0.6927983464168281</v>
       </c>
       <c r="J6" t="n">
-        <v>0.3732391460051863</v>
+        <v>0.499637322800165</v>
       </c>
       <c r="K6" t="n">
-        <v>0.6514483409120799</v>
+        <v>0.6561596113299912</v>
       </c>
       <c r="L6" t="n">
         <v>0.761032490251111</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8238788466306596</v>
+        <v>0.4073430323889371</v>
       </c>
       <c r="N6" t="n">
         <v>0.2975605320903996</v>
       </c>
       <c r="O6" t="n">
-        <v>0.2701953994556955</v>
+        <v>0.3617692475965423</v>
       </c>
     </row>
     <row r="7">
@@ -801,31 +801,31 @@
         <v>-0.5408945326843502</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1835360385980752</v>
+        <v>0.2339345087460386</v>
       </c>
       <c r="H7" t="n">
         <v>0.4236113941885588</v>
       </c>
       <c r="I7" t="n">
-        <v>0.2453960502847712</v>
+        <v>0.2340170282194848</v>
       </c>
       <c r="J7" t="n">
-        <v>0.317125961308623</v>
+        <v>0.2211828025353424</v>
       </c>
       <c r="K7" t="n">
-        <v>0.7231378696807279</v>
+        <v>0.7255852489729558</v>
       </c>
       <c r="L7" t="n">
         <v>0.2468949326188494</v>
       </c>
       <c r="M7" t="n">
-        <v>0.3064428914449464</v>
+        <v>0.3388181849359906</v>
       </c>
       <c r="N7" t="n">
         <v>0.4560734139035991</v>
       </c>
       <c r="O7" t="n">
-        <v>0.3637502277382452</v>
+        <v>0.4219135222636656</v>
       </c>
     </row>
     <row r="8">
@@ -854,31 +854,31 @@
         <v>-1.108408340134865</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4973232449006817</v>
+        <v>0.5218584798125326</v>
       </c>
       <c r="H8" t="n">
         <v>0.405038482153842</v>
       </c>
       <c r="I8" t="n">
-        <v>0.3790370200892494</v>
+        <v>0.4269770201465697</v>
       </c>
       <c r="J8" t="n">
-        <v>0.5231377588429943</v>
+        <v>0.3478409681710704</v>
       </c>
       <c r="K8" t="n">
-        <v>0.6696433691308527</v>
+        <v>0.6713204581193503</v>
       </c>
       <c r="L8" t="n">
         <v>0.2507766209342789</v>
       </c>
       <c r="M8" t="n">
-        <v>0.3158300361384082</v>
+        <v>0.2777087986815598</v>
       </c>
       <c r="N8" t="n">
         <v>1.360616366279739</v>
       </c>
       <c r="O8" t="n">
-        <v>0.2577242353421769</v>
+        <v>0.342433425251829</v>
       </c>
     </row>
     <row r="9">
@@ -907,31 +907,31 @@
         <v>-1.376343170365185</v>
       </c>
       <c r="G9" t="n">
-        <v>0.7033945816123645</v>
+        <v>0.7166187989284143</v>
       </c>
       <c r="H9" t="n">
         <v>0.5023272157123083</v>
       </c>
       <c r="I9" t="n">
-        <v>0.5157075170026092</v>
+        <v>0.5093922466907995</v>
       </c>
       <c r="J9" t="n">
-        <v>0.3631129084209323</v>
+        <v>0.3622002300607757</v>
       </c>
       <c r="K9" t="n">
-        <v>0.6491187529046184</v>
+        <v>0.6506051046548891</v>
       </c>
       <c r="L9" t="n">
         <v>0.4047421519898545</v>
       </c>
       <c r="M9" t="n">
-        <v>0.4229354330200015</v>
+        <v>0.3202129035300945</v>
       </c>
       <c r="N9" t="n">
         <v>0.4019985060935735</v>
       </c>
       <c r="O9" t="n">
-        <v>0.5020867057776736</v>
+        <v>0.4218013207848155</v>
       </c>
     </row>
     <row r="10">
@@ -960,31 +960,31 @@
         <v>0.682215902775701</v>
       </c>
       <c r="G10" t="n">
-        <v>0.7479649714071849</v>
+        <v>0.6024356727075499</v>
       </c>
       <c r="H10" t="n">
         <v>0.7680070405969008</v>
       </c>
       <c r="I10" t="n">
-        <v>0.7106870727591934</v>
+        <v>0.7197157884090679</v>
       </c>
       <c r="J10" t="n">
-        <v>1.211767670331493</v>
+        <v>1.156404960599048</v>
       </c>
       <c r="K10" t="n">
-        <v>0.8603128679894412</v>
+        <v>0.8599616982087048</v>
       </c>
       <c r="L10" t="n">
         <v>0.9248526397991005</v>
       </c>
       <c r="M10" t="n">
-        <v>0.8947336954027379</v>
+        <v>1.052450656498203</v>
       </c>
       <c r="N10" t="n">
         <v>0.9473220559791302</v>
       </c>
       <c r="O10" t="n">
-        <v>0.8619649652239814</v>
+        <v>0.7045524970028708</v>
       </c>
     </row>
     <row r="11">
@@ -1013,31 +1013,31 @@
         <v>-2.675784227426882</v>
       </c>
       <c r="G11" t="n">
-        <v>1.908086887498878</v>
+        <v>1.862080997882652</v>
       </c>
       <c r="H11" t="n">
         <v>2.024083403979535</v>
       </c>
       <c r="I11" t="n">
-        <v>1.632900237250358</v>
+        <v>1.584663472020739</v>
       </c>
       <c r="J11" t="n">
-        <v>1.43942572639359</v>
+        <v>1.674600097977642</v>
       </c>
       <c r="K11" t="n">
-        <v>1.137008838340316</v>
+        <v>1.146178872540844</v>
       </c>
       <c r="L11" t="n">
         <v>1.460016380468639</v>
       </c>
       <c r="M11" t="n">
-        <v>1.397911311307754</v>
+        <v>1.20733943113395</v>
       </c>
       <c r="N11" t="n">
         <v>1.363402992851606</v>
       </c>
       <c r="O11" t="n">
-        <v>1.781570975683298</v>
+        <v>1.880874184483762</v>
       </c>
     </row>
     <row r="12">
@@ -1066,31 +1066,31 @@
         <v>-3.279926069822571</v>
       </c>
       <c r="G12" t="n">
-        <v>2.501348068193407</v>
+        <v>2.439748241263175</v>
       </c>
       <c r="H12" t="n">
         <v>1.647852170413031</v>
       </c>
       <c r="I12" t="n">
-        <v>2.19988703619734</v>
+        <v>2.156943198439215</v>
       </c>
       <c r="J12" t="n">
-        <v>1.359705950441971</v>
+        <v>1.086398644454755</v>
       </c>
       <c r="K12" t="n">
-        <v>1.716032575595976</v>
+        <v>1.72620320147629</v>
       </c>
       <c r="L12" t="n">
         <v>2.493812880028518</v>
       </c>
       <c r="M12" t="n">
-        <v>2.497274518659028</v>
+        <v>1.801475110378239</v>
       </c>
       <c r="N12" t="n">
         <v>1.327829824078715</v>
       </c>
       <c r="O12" t="n">
-        <v>1.280722459496094</v>
+        <v>1.419224967255788</v>
       </c>
     </row>
     <row r="13">
@@ -1119,31 +1119,31 @@
         <v>-3.043658077184164</v>
       </c>
       <c r="G13" t="n">
-        <v>2.256093296313761</v>
+        <v>2.209278834976443</v>
       </c>
       <c r="H13" t="n">
         <v>2.523716706927503</v>
       </c>
       <c r="I13" t="n">
-        <v>1.907551770133102</v>
+        <v>1.941628516358671</v>
       </c>
       <c r="J13" t="n">
-        <v>0.8942079654647338</v>
+        <v>0.8538861526896857</v>
       </c>
       <c r="K13" t="n">
-        <v>1.438217552698942</v>
+        <v>1.450516649476119</v>
       </c>
       <c r="L13" t="n">
         <v>1.52525383094681</v>
       </c>
       <c r="M13" t="n">
-        <v>1.381777342852355</v>
+        <v>1.565679653725108</v>
       </c>
       <c r="N13" t="n">
         <v>1.452233062266469</v>
       </c>
       <c r="O13" t="n">
-        <v>1.585363953320531</v>
+        <v>1.348002749600517</v>
       </c>
     </row>
     <row r="14">
@@ -1172,19 +1172,19 @@
         <v>-1.445206376294113</v>
       </c>
       <c r="G14" t="n">
-        <v>0.6867238562624493</v>
+        <v>0.5594845440567042</v>
       </c>
       <c r="H14" t="n">
         <v>0.4604587076533443</v>
       </c>
       <c r="I14" t="n">
-        <v>0.5843235062595977</v>
+        <v>0.6066304995240968</v>
       </c>
       <c r="J14" t="n">
-        <v>0.6094300982767857</v>
+        <v>0.5877663687395481</v>
       </c>
       <c r="K14" t="n">
-        <v>0.6365388387728355</v>
+        <v>0.6295399261422575</v>
       </c>
       <c r="L14" t="n">
         <v>0.7607079796455161</v>
@@ -1196,7 +1196,7 @@
         <v>0.470865186591349</v>
       </c>
       <c r="O14" t="n">
-        <v>0.4207125328800009</v>
+        <v>0.4781814993678736</v>
       </c>
     </row>
     <row r="15">
@@ -1225,31 +1225,31 @@
         <v>-0.8566358209542351</v>
       </c>
       <c r="G15" t="n">
-        <v>0.2249613729747264</v>
+        <v>0.2330449601877848</v>
       </c>
       <c r="H15" t="n">
         <v>0.3501322276321447</v>
       </c>
       <c r="I15" t="n">
-        <v>0.3088381086480307</v>
+        <v>0.3116334807214568</v>
       </c>
       <c r="J15" t="n">
-        <v>0.3083983795455995</v>
+        <v>0.3074736838596404</v>
       </c>
       <c r="K15" t="n">
-        <v>0.6827231335591717</v>
+        <v>0.6770930661394439</v>
       </c>
       <c r="L15" t="n">
         <v>0.2642061494722038</v>
       </c>
       <c r="M15" t="n">
-        <v>0.2425031336174752</v>
+        <v>0.4158797868320672</v>
       </c>
       <c r="N15" t="n">
         <v>0.1992275815932099</v>
       </c>
       <c r="O15" t="n">
-        <v>0.3615852854241215</v>
+        <v>0.2546694730609776</v>
       </c>
     </row>
     <row r="16">
@@ -1278,31 +1278,31 @@
         <v>0.6888498721555987</v>
       </c>
       <c r="G16" t="n">
-        <v>0.8995919993839062</v>
+        <v>0.8301659967663215</v>
       </c>
       <c r="H16" t="n">
         <v>0.5982532228449902</v>
       </c>
       <c r="I16" t="n">
-        <v>0.6513132827978889</v>
+        <v>0.6487811912476636</v>
       </c>
       <c r="J16" t="n">
-        <v>0.5971123275775557</v>
+        <v>0.6940797106820545</v>
       </c>
       <c r="K16" t="n">
-        <v>0.8672487694980853</v>
+        <v>0.8630725898716562</v>
       </c>
       <c r="L16" t="n">
         <v>0.7582499204106015</v>
       </c>
       <c r="M16" t="n">
-        <v>0.7930003753413062</v>
+        <v>0.5047890299838209</v>
       </c>
       <c r="N16" t="n">
         <v>0.5239253995593095</v>
       </c>
       <c r="O16" t="n">
-        <v>0.4316344809548303</v>
+        <v>0.6396820294032204</v>
       </c>
     </row>
     <row r="17">
@@ -1331,31 +1331,31 @@
         <v>-0.2772595486131353</v>
       </c>
       <c r="G17" t="n">
-        <v>0.1466143393637357</v>
+        <v>0.2217847782587894</v>
       </c>
       <c r="H17" t="n">
         <v>0.2427927373398645</v>
       </c>
       <c r="I17" t="n">
-        <v>0.2593182703146905</v>
+        <v>0.2636546328138152</v>
       </c>
       <c r="J17" t="n">
-        <v>0.2206346614768642</v>
+        <v>0.2897748490341038</v>
       </c>
       <c r="K17" t="n">
-        <v>0.7491304172183106</v>
+        <v>0.7429760596458208</v>
       </c>
       <c r="L17" t="n">
         <v>0.249656579786262</v>
       </c>
       <c r="M17" t="n">
-        <v>0.2530589298829756</v>
+        <v>0.2408162117359516</v>
       </c>
       <c r="N17" t="n">
         <v>0.3565567727022813</v>
       </c>
       <c r="O17" t="n">
-        <v>0.287571406486541</v>
+        <v>0.2508553772214462</v>
       </c>
     </row>
     <row r="18">
@@ -1384,31 +1384,31 @@
         <v>-0.6640387420841678</v>
       </c>
       <c r="G18" t="n">
-        <v>0.1457747067738713</v>
+        <v>0.1914774984736885</v>
       </c>
       <c r="H18" t="n">
         <v>0.2000190373909477</v>
       </c>
       <c r="I18" t="n">
-        <v>0.2678530817174114</v>
+        <v>0.2688765158883483</v>
       </c>
       <c r="J18" t="n">
-        <v>0.2726119882882719</v>
+        <v>0.2682123033864766</v>
       </c>
       <c r="K18" t="n">
-        <v>0.7049968141213758</v>
+        <v>0.6990447305795762</v>
       </c>
       <c r="L18" t="n">
         <v>0.3501809421973322</v>
       </c>
       <c r="M18" t="n">
-        <v>0.3200328049152458</v>
+        <v>0.3146403115582309</v>
       </c>
       <c r="N18" t="n">
         <v>0.1522845121567541</v>
       </c>
       <c r="O18" t="n">
-        <v>0.246648119118392</v>
+        <v>0.2349082125301026</v>
       </c>
     </row>
     <row r="19">
@@ -1437,31 +1437,31 @@
         <v>-1.107400879733716</v>
       </c>
       <c r="G19" t="n">
-        <v>0.3989672454104016</v>
+        <v>0.347339177607937</v>
       </c>
       <c r="H19" t="n">
         <v>0.6492923955702398</v>
       </c>
       <c r="I19" t="n">
-        <v>0.4164466168993504</v>
+        <v>0.4181706787803032</v>
       </c>
       <c r="J19" t="n">
-        <v>0.4200516661991275</v>
+        <v>0.3914062694776969</v>
       </c>
       <c r="K19" t="n">
-        <v>0.6602741132588557</v>
+        <v>0.654271755691425</v>
       </c>
       <c r="L19" t="n">
         <v>0.3287397902889628</v>
       </c>
       <c r="M19" t="n">
-        <v>0.2864615568055187</v>
+        <v>0.5703237083467829</v>
       </c>
       <c r="N19" t="n">
         <v>0.8621662154782719</v>
       </c>
       <c r="O19" t="n">
-        <v>0.455805940294726</v>
+        <v>0.3521912712262327</v>
       </c>
     </row>
     <row r="20">
@@ -1490,31 +1490,31 @@
         <v>-0.3227047909551708</v>
       </c>
       <c r="G20" t="n">
-        <v>0.1354600296634546</v>
+        <v>0.2094056339755848</v>
       </c>
       <c r="H20" t="n">
         <v>0.3273011022142788</v>
       </c>
       <c r="I20" t="n">
-        <v>0.2554867508737053</v>
+        <v>0.2354635038536856</v>
       </c>
       <c r="J20" t="n">
-        <v>0.2557733632398181</v>
+        <v>0.2766604675248611</v>
       </c>
       <c r="K20" t="n">
-        <v>0.7442212941837092</v>
+        <v>0.7388328882395838</v>
       </c>
       <c r="L20" t="n">
         <v>0.2633574399511397</v>
       </c>
       <c r="M20" t="n">
-        <v>0.2583196211572187</v>
+        <v>0.2410705361697636</v>
       </c>
       <c r="N20" t="n">
         <v>0.409735489923611</v>
       </c>
       <c r="O20" t="n">
-        <v>0.2356974117721257</v>
+        <v>0.2784748908302692</v>
       </c>
     </row>
     <row r="21">
@@ -1543,31 +1543,31 @@
         <v>-0.09636687889850903</v>
       </c>
       <c r="G21" t="n">
-        <v>0.2267949093803922</v>
+        <v>0.2803610324661884</v>
       </c>
       <c r="H21" t="n">
         <v>0.3937130849667385</v>
       </c>
       <c r="I21" t="n">
-        <v>0.285327446919927</v>
+        <v>0.2862780413145777</v>
       </c>
       <c r="J21" t="n">
-        <v>0.2716949772403596</v>
+        <v>0.3010800891458826</v>
       </c>
       <c r="K21" t="n">
-        <v>0.7708249174827722</v>
+        <v>0.765275624254403</v>
       </c>
       <c r="L21" t="n">
         <v>0.3182117492692488</v>
       </c>
       <c r="M21" t="n">
-        <v>0.3387816464005041</v>
+        <v>0.2558664925255891</v>
       </c>
       <c r="N21" t="n">
         <v>0.3683983310593923</v>
       </c>
       <c r="O21" t="n">
-        <v>0.2429148486469702</v>
+        <v>0.2579204342093958</v>
       </c>
     </row>
     <row r="22">
@@ -1596,31 +1596,31 @@
         <v>0.298650936879099</v>
       </c>
       <c r="G22" t="n">
-        <v>0.5225525424708766</v>
+        <v>0.5121723496042556</v>
       </c>
       <c r="H22" t="n">
         <v>0.3590113314252176</v>
       </c>
       <c r="I22" t="n">
-        <v>0.4658208271456155</v>
+        <v>0.4356322078536043</v>
       </c>
       <c r="J22" t="n">
-        <v>0.4061345448163691</v>
+        <v>0.4601860729658694</v>
       </c>
       <c r="K22" t="n">
-        <v>0.8172184306943747</v>
+        <v>0.8114704239280416</v>
       </c>
       <c r="L22" t="n">
         <v>0.3728421429240272</v>
       </c>
       <c r="M22" t="n">
-        <v>0.3891474675718513</v>
+        <v>0.3451142342961169</v>
       </c>
       <c r="N22" t="n">
         <v>0.3509718394356887</v>
       </c>
       <c r="O22" t="n">
-        <v>0.4765845474584297</v>
+        <v>0.4130297764902056</v>
       </c>
     </row>
     <row r="23">
@@ -1649,31 +1649,31 @@
         <v>0.1912005181776173</v>
       </c>
       <c r="G23" t="n">
-        <v>0.4307327311930538</v>
+        <v>0.4364556868657948</v>
       </c>
       <c r="H23" t="n">
         <v>0.3093084264703347</v>
       </c>
       <c r="I23" t="n">
-        <v>0.3924712344125866</v>
+        <v>0.3493979849081216</v>
       </c>
       <c r="J23" t="n">
-        <v>0.3287175575616966</v>
+        <v>0.3934539751368294</v>
       </c>
       <c r="K23" t="n">
-        <v>0.8050267492037859</v>
+        <v>0.7988085137592207</v>
       </c>
       <c r="L23" t="n">
         <v>0.4040927187333575</v>
       </c>
       <c r="M23" t="n">
-        <v>0.4199077512859042</v>
+        <v>0.3138012994850925</v>
       </c>
       <c r="N23" t="n">
         <v>0.3428268670094803</v>
       </c>
       <c r="O23" t="n">
-        <v>0.3782731358492514</v>
+        <v>0.3787537548649644</v>
       </c>
     </row>
     <row r="24">
@@ -1702,31 +1702,31 @@
         <v>-1.451663169588896</v>
       </c>
       <c r="G24" t="n">
-        <v>0.7004571664461332</v>
+        <v>0.5717124853322739</v>
       </c>
       <c r="H24" t="n">
         <v>0.7299061371819893</v>
       </c>
       <c r="I24" t="n">
-        <v>0.6602879757944289</v>
+        <v>0.6146609287772477</v>
       </c>
       <c r="J24" t="n">
-        <v>0.6774542405794702</v>
+        <v>0.6155464648401392</v>
       </c>
       <c r="K24" t="n">
-        <v>0.6416836812496051</v>
+        <v>0.635463278372507</v>
       </c>
       <c r="L24" t="n">
         <v>0.6522510810891509</v>
       </c>
       <c r="M24" t="n">
-        <v>0.715972759160959</v>
+        <v>0.7963150737309872</v>
       </c>
       <c r="N24" t="n">
         <v>1.048797355368231</v>
       </c>
       <c r="O24" t="n">
-        <v>0.7559154860408654</v>
+        <v>0.5675910868027001</v>
       </c>
     </row>
     <row r="25">
@@ -1755,31 +1755,31 @@
         <v>-0.1203686219198782</v>
       </c>
       <c r="G25" t="n">
-        <v>0.2107353164460222</v>
+        <v>0.2665965921611493</v>
       </c>
       <c r="H25" t="n">
         <v>0.3881895738973692</v>
       </c>
       <c r="I25" t="n">
-        <v>0.2863314085846553</v>
+        <v>0.2853736705985076</v>
       </c>
       <c r="J25" t="n">
-        <v>0.358706471488202</v>
+        <v>0.317474040658008</v>
       </c>
       <c r="K25" t="n">
-        <v>0.7687538909888941</v>
+        <v>0.7631565096809071</v>
       </c>
       <c r="L25" t="n">
         <v>0.2981247450723863</v>
       </c>
       <c r="M25" t="n">
-        <v>0.2505360817808703</v>
+        <v>0.2535143217094947</v>
       </c>
       <c r="N25" t="n">
         <v>0.1597775121464154</v>
       </c>
       <c r="O25" t="n">
-        <v>0.33892755016608</v>
+        <v>0.3574792898582413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mejora de codigo, aplicacion de densidades vs densidades con ECRPS y graficación para simulacion base
</commit_message>
<xml_diff>
--- a/codigo_final_organizado/Simulaciones/NO_lineal_estacionario/resultados_2_ESCENARIOS_SETAR.xlsx
+++ b/codigo_final_organizado/Simulaciones/NO_lineal_estacionario/resultados_2_ESCENARIOS_SETAR.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>proces_simulacion</t>
+          <t>Config</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -451,62 +451,57 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Distribución</t>
+          <t>Dist</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Varianza error</t>
+          <t>Var</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Valor_Observado</t>
+          <t>Block Bootstrapping</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Sieve Bootstrap</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>LSPM</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>LSPMW</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>AREPD</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>MCPS</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>AV-MCPS</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Block Bootstrapping</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>DeepAR</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>EnCQR-LSTM</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>LSPM</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>LSPMW</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>MCPS</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Sieve Bootstrap</t>
         </is>
       </c>
     </row>
@@ -533,34 +528,31 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.1576794063200361</v>
+        <v>0.6369513500959092</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1920478055701966</v>
+        <v>0.5843994421329943</v>
       </c>
       <c r="H2" t="n">
-        <v>0.3231141130128508</v>
+        <v>0.570469362795984</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2931153080917904</v>
+        <v>0.570840921275085</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2240828618179215</v>
+        <v>0.6533329303549965</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7594023393015787</v>
+        <v>0.8549203449787076</v>
       </c>
       <c r="L2" t="n">
-        <v>0.4906307953793766</v>
+        <v>0.7161690003526351</v>
       </c>
       <c r="M2" t="n">
-        <v>0.4843090051523787</v>
+        <v>0.6283347284026712</v>
       </c>
       <c r="N2" t="n">
-        <v>0.4134802190192442</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0.3018189596204621</v>
+        <v>0.8774877686127051</v>
       </c>
     </row>
     <row r="3">
@@ -586,34 +578,31 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9771613873707746</v>
+        <v>0.7682142964308963</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8440802290461885</v>
+        <v>0.5875887580573944</v>
       </c>
       <c r="H3" t="n">
-        <v>0.8971380629950961</v>
+        <v>0.9091143611602889</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9486587492742637</v>
+        <v>1.093086879111845</v>
       </c>
       <c r="J3" t="n">
-        <v>0.8030715638437396</v>
+        <v>0.7846454750213733</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9191225853813544</v>
+        <v>0.6182420795381399</v>
       </c>
       <c r="L3" t="n">
-        <v>0.963195275359668</v>
+        <v>0.8092470716527327</v>
       </c>
       <c r="M3" t="n">
-        <v>1.36548478079573</v>
+        <v>0.730450496981359</v>
       </c>
       <c r="N3" t="n">
-        <v>1.429328977467928</v>
-      </c>
-      <c r="O3" t="n">
-        <v>1.147772757933678</v>
+        <v>0.8793067227491869</v>
       </c>
     </row>
     <row r="4">
@@ -639,34 +628,31 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.7514160756679074</v>
+        <v>0.5655028703433915</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3205563771652512</v>
+        <v>0.5656516677990023</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3209898055826283</v>
+        <v>0.6579954765286115</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2765914636051733</v>
+        <v>0.652997466551634</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4265827512322169</v>
+        <v>0.5706582279067366</v>
       </c>
       <c r="K4" t="n">
-        <v>0.7020093069832635</v>
+        <v>0.6582565985149048</v>
       </c>
       <c r="L4" t="n">
-        <v>0.2439267986604944</v>
+        <v>0.6241631250665416</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2683431762503036</v>
+        <v>0.5673764652125339</v>
       </c>
       <c r="N4" t="n">
-        <v>0.2231246744978527</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.6361204696781061</v>
+        <v>0.8285478870291892</v>
       </c>
     </row>
     <row r="5">
@@ -692,34 +678,31 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>-2.218401011803054</v>
+        <v>0.5871901013957525</v>
       </c>
       <c r="G5" t="n">
-        <v>1.438599549706423</v>
+        <v>0.5654217395649502</v>
       </c>
       <c r="H5" t="n">
-        <v>1.604614918095754</v>
+        <v>0.5718470472866304</v>
       </c>
       <c r="I5" t="n">
-        <v>1.227672168773977</v>
+        <v>0.5837226012779879</v>
       </c>
       <c r="J5" t="n">
-        <v>1.902151601688216</v>
+        <v>0.5875137066800068</v>
       </c>
       <c r="K5" t="n">
-        <v>0.8321536731438657</v>
+        <v>0.7210538059920016</v>
       </c>
       <c r="L5" t="n">
-        <v>1.738231484259985</v>
+        <v>0.5974819202697724</v>
       </c>
       <c r="M5" t="n">
-        <v>0.7941101279597217</v>
+        <v>0.5979892408691407</v>
       </c>
       <c r="N5" t="n">
-        <v>0.8386608194390208</v>
-      </c>
-      <c r="O5" t="n">
-        <v>1.164045658562616</v>
+        <v>0.850878739895186</v>
       </c>
     </row>
     <row r="6">
@@ -745,34 +728,31 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>-1.618314180070109</v>
+        <v>0.6491540140440122</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9131169179845734</v>
+        <v>0.6697446540368869</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6015351021412634</v>
+        <v>0.6239498082976067</v>
       </c>
       <c r="I6" t="n">
-        <v>0.6927983464168281</v>
+        <v>0.5680768436293515</v>
       </c>
       <c r="J6" t="n">
-        <v>0.499637322800165</v>
+        <v>0.6861917308243309</v>
       </c>
       <c r="K6" t="n">
-        <v>0.6528774572507436</v>
+        <v>0.6425446912940814</v>
       </c>
       <c r="L6" t="n">
-        <v>0.761032490251111</v>
+        <v>0.7035799170340037</v>
       </c>
       <c r="M6" t="n">
-        <v>0.393751305815818</v>
+        <v>0.6405699624203186</v>
       </c>
       <c r="N6" t="n">
-        <v>0.2975605320903996</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.3617692475965423</v>
+        <v>0.8936736347922928</v>
       </c>
     </row>
     <row r="7">
@@ -798,34 +778,31 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.5408945326843502</v>
+        <v>0.5894449602282741</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2339345087460386</v>
+        <v>0.8230185070006231</v>
       </c>
       <c r="H7" t="n">
-        <v>0.4236113941885588</v>
+        <v>0.586411766223163</v>
       </c>
       <c r="I7" t="n">
-        <v>0.2340170282194848</v>
+        <v>0.7018933605115637</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2211828025353424</v>
+        <v>0.5903694533282057</v>
       </c>
       <c r="K7" t="n">
-        <v>0.7224392769862428</v>
+        <v>0.6938511040699863</v>
       </c>
       <c r="L7" t="n">
-        <v>0.2468949326188494</v>
+        <v>1.004307895169496</v>
       </c>
       <c r="M7" t="n">
-        <v>0.3260101172571158</v>
+        <v>0.5871122686892942</v>
       </c>
       <c r="N7" t="n">
-        <v>0.4560734139035991</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.4219135222636656</v>
+        <v>0.8400430956102833</v>
       </c>
     </row>
     <row r="8">
@@ -851,34 +828,31 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>-1.108408340134865</v>
+        <v>0.866279039966514</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5218584798125326</v>
+        <v>0.5734746947094902</v>
       </c>
       <c r="H8" t="n">
-        <v>0.405038482153842</v>
+        <v>1.389276288467841</v>
       </c>
       <c r="I8" t="n">
-        <v>0.4269770201465697</v>
+        <v>1.216497922655282</v>
       </c>
       <c r="J8" t="n">
-        <v>0.3478409681710704</v>
+        <v>0.8693556945192348</v>
       </c>
       <c r="K8" t="n">
-        <v>0.6689448310006813</v>
+        <v>0.7326250492836474</v>
       </c>
       <c r="L8" t="n">
-        <v>0.2507766209342789</v>
+        <v>0.9160571857826871</v>
       </c>
       <c r="M8" t="n">
-        <v>0.2490139508291321</v>
+        <v>0.8188226430512602</v>
       </c>
       <c r="N8" t="n">
-        <v>1.360616366279739</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0.342433425251829</v>
+        <v>0.9052844873369854</v>
       </c>
     </row>
     <row r="9">
@@ -904,34 +878,31 @@
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>-1.376343170365185</v>
+        <v>0.7084516708508127</v>
       </c>
       <c r="G9" t="n">
-        <v>0.7166187989284143</v>
+        <v>0.5852166589566348</v>
       </c>
       <c r="H9" t="n">
-        <v>0.5023272157123083</v>
+        <v>0.5567462903302045</v>
       </c>
       <c r="I9" t="n">
-        <v>0.5093922466907995</v>
+        <v>1.030104100435964</v>
       </c>
       <c r="J9" t="n">
-        <v>0.3622002300607757</v>
+        <v>0.7335859563576617</v>
       </c>
       <c r="K9" t="n">
-        <v>0.6495829054855937</v>
+        <v>0.7304313654266728</v>
       </c>
       <c r="L9" t="n">
-        <v>0.4047421519898545</v>
+        <v>0.7194836693236835</v>
       </c>
       <c r="M9" t="n">
-        <v>0.29563841016148</v>
+        <v>0.6823386964956435</v>
       </c>
       <c r="N9" t="n">
-        <v>0.4019985060935735</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0.4218013207848155</v>
+        <v>0.8565212200005967</v>
       </c>
     </row>
     <row r="10">
@@ -957,34 +928,31 @@
         <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.682215902775701</v>
+        <v>0.5919218337762049</v>
       </c>
       <c r="G10" t="n">
-        <v>0.6024356727075499</v>
+        <v>0.5906312704983701</v>
       </c>
       <c r="H10" t="n">
-        <v>0.7680070405969008</v>
+        <v>0.6732591212121318</v>
       </c>
       <c r="I10" t="n">
-        <v>0.7197157884090679</v>
+        <v>0.629151650987046</v>
       </c>
       <c r="J10" t="n">
-        <v>1.156404960599048</v>
+        <v>0.5956020494428479</v>
       </c>
       <c r="K10" t="n">
-        <v>0.8572950184359456</v>
+        <v>0.8982715979309793</v>
       </c>
       <c r="L10" t="n">
-        <v>0.9248526397991005</v>
+        <v>0.6249703065285882</v>
       </c>
       <c r="M10" t="n">
-        <v>1.08648801352677</v>
+        <v>0.5942904237517793</v>
       </c>
       <c r="N10" t="n">
-        <v>0.9473220559791302</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0.7045524970028708</v>
+        <v>0.8440793537434786</v>
       </c>
     </row>
     <row r="11">
@@ -1010,34 +978,31 @@
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>-2.675784227426882</v>
+        <v>0.7125432013468992</v>
       </c>
       <c r="G11" t="n">
-        <v>1.862080997882652</v>
+        <v>0.5765485154551552</v>
       </c>
       <c r="H11" t="n">
-        <v>2.024083403979535</v>
+        <v>0.8241314124589615</v>
       </c>
       <c r="I11" t="n">
-        <v>1.584663472020739</v>
+        <v>0.9439419395309855</v>
       </c>
       <c r="J11" t="n">
-        <v>1.674600097977642</v>
+        <v>0.6868509931530272</v>
       </c>
       <c r="K11" t="n">
-        <v>1.166168156856927</v>
+        <v>0.7833991882374014</v>
       </c>
       <c r="L11" t="n">
-        <v>1.460016380468639</v>
+        <v>0.7115120218891509</v>
       </c>
       <c r="M11" t="n">
-        <v>1.193618170623214</v>
+        <v>0.6467199027169138</v>
       </c>
       <c r="N11" t="n">
-        <v>1.363402992851606</v>
-      </c>
-      <c r="O11" t="n">
-        <v>1.880874184483762</v>
+        <v>0.8431892721908881</v>
       </c>
     </row>
     <row r="12">
@@ -1063,34 +1028,31 @@
         <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>-3.279926069822571</v>
+        <v>0.6271611672714793</v>
       </c>
       <c r="G12" t="n">
-        <v>2.439748241263175</v>
+        <v>0.5788479493160956</v>
       </c>
       <c r="H12" t="n">
-        <v>1.647852170413031</v>
+        <v>0.8814978351959203</v>
       </c>
       <c r="I12" t="n">
-        <v>2.156943198439215</v>
+        <v>0.5767767344497744</v>
       </c>
       <c r="J12" t="n">
-        <v>1.086398644454755</v>
+        <v>0.6693722492930013</v>
       </c>
       <c r="K12" t="n">
-        <v>1.749765316945811</v>
+        <v>0.8133305091970324</v>
       </c>
       <c r="L12" t="n">
-        <v>2.493812880028518</v>
+        <v>0.7891414364067056</v>
       </c>
       <c r="M12" t="n">
-        <v>1.778185541566537</v>
+        <v>0.6596160004108806</v>
       </c>
       <c r="N12" t="n">
-        <v>1.327829824078715</v>
-      </c>
-      <c r="O12" t="n">
-        <v>1.419224967255788</v>
+        <v>0.8859857166476947</v>
       </c>
     </row>
     <row r="13">
@@ -1116,34 +1078,31 @@
         <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>-3.043658077184164</v>
+        <v>0.5990583492553717</v>
       </c>
       <c r="G13" t="n">
-        <v>2.209278834976443</v>
+        <v>0.5528112836089469</v>
       </c>
       <c r="H13" t="n">
-        <v>2.523716706927503</v>
+        <v>0.5600460369563607</v>
       </c>
       <c r="I13" t="n">
-        <v>1.941628516358671</v>
+        <v>0.5516873544602805</v>
       </c>
       <c r="J13" t="n">
-        <v>0.8538861526896857</v>
+        <v>0.6265093932357716</v>
       </c>
       <c r="K13" t="n">
-        <v>1.481843511032632</v>
+        <v>1.469510826562523</v>
       </c>
       <c r="L13" t="n">
-        <v>1.52525383094681</v>
+        <v>1.288047325402368</v>
       </c>
       <c r="M13" t="n">
-        <v>1.545785333250495</v>
+        <v>0.6033556026092327</v>
       </c>
       <c r="N13" t="n">
-        <v>1.452233062266469</v>
-      </c>
-      <c r="O13" t="n">
-        <v>1.348002749600517</v>
+        <v>0.873602431543</v>
       </c>
     </row>
     <row r="14">
@@ -1169,34 +1128,31 @@
         <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>-1.445206376294113</v>
+        <v>0.5833981083963058</v>
       </c>
       <c r="G14" t="n">
-        <v>0.5594845440567042</v>
+        <v>0.5762481950672734</v>
       </c>
       <c r="H14" t="n">
-        <v>0.4604587076533443</v>
+        <v>0.5863248494721115</v>
       </c>
       <c r="I14" t="n">
-        <v>0.6066304995240968</v>
+        <v>0.5757911765018415</v>
       </c>
       <c r="J14" t="n">
-        <v>0.5877663687395481</v>
+        <v>0.6074554900455291</v>
       </c>
       <c r="K14" t="n">
-        <v>0.633761718521524</v>
+        <v>0.826983955591566</v>
       </c>
       <c r="L14" t="n">
-        <v>0.7607079796455161</v>
+        <v>0.6633086149499661</v>
       </c>
       <c r="M14" t="n">
-        <v>0.7354779328243995</v>
+        <v>0.5818056121320607</v>
       </c>
       <c r="N14" t="n">
-        <v>0.470865186591349</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0.4781814993678736</v>
+        <v>0.8176024116982845</v>
       </c>
     </row>
     <row r="15">
@@ -1222,34 +1178,31 @@
         <v>1</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.8566358209542351</v>
+        <v>0.6332534597162516</v>
       </c>
       <c r="G15" t="n">
-        <v>0.2330449601877848</v>
+        <v>0.5998194372902358</v>
       </c>
       <c r="H15" t="n">
-        <v>0.3501322276321447</v>
+        <v>0.6455339243162069</v>
       </c>
       <c r="I15" t="n">
-        <v>0.3116334807214568</v>
+        <v>0.6554499564311369</v>
       </c>
       <c r="J15" t="n">
-        <v>0.3074736838596404</v>
+        <v>0.7355551910426364</v>
       </c>
       <c r="K15" t="n">
-        <v>0.6813228819063484</v>
+        <v>0.8649617968662444</v>
       </c>
       <c r="L15" t="n">
-        <v>0.2642061494722038</v>
+        <v>0.7112451215453883</v>
       </c>
       <c r="M15" t="n">
-        <v>0.3941211788185811</v>
+        <v>0.6148501938233483</v>
       </c>
       <c r="N15" t="n">
-        <v>0.1992275815932099</v>
-      </c>
-      <c r="O15" t="n">
-        <v>0.2546694730609776</v>
+        <v>0.8236548418040509</v>
       </c>
     </row>
     <row r="16">
@@ -1275,34 +1228,31 @@
         <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>0.6888498721555987</v>
+        <v>0.5670396182421353</v>
       </c>
       <c r="G16" t="n">
-        <v>0.8301659967663215</v>
+        <v>0.5592416729828991</v>
       </c>
       <c r="H16" t="n">
-        <v>0.5982532228449902</v>
+        <v>0.577067856635735</v>
       </c>
       <c r="I16" t="n">
-        <v>0.6487811912476636</v>
+        <v>0.5597833288966785</v>
       </c>
       <c r="J16" t="n">
-        <v>0.6940797106820545</v>
+        <v>0.5985497539529903</v>
       </c>
       <c r="K16" t="n">
-        <v>0.8671805920593697</v>
+        <v>0.5881596631715506</v>
       </c>
       <c r="L16" t="n">
-        <v>0.7582499204106015</v>
+        <v>0.5953917086742714</v>
       </c>
       <c r="M16" t="n">
-        <v>0.5340462395551343</v>
+        <v>0.5712401996326767</v>
       </c>
       <c r="N16" t="n">
-        <v>0.5239253995593095</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0.6396820294032204</v>
+        <v>0.8005371384073549</v>
       </c>
     </row>
     <row r="17">
@@ -1328,34 +1278,31 @@
         <v>1</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.2772595486131353</v>
+        <v>0.5810647307474653</v>
       </c>
       <c r="G17" t="n">
-        <v>0.2217847782587894</v>
+        <v>0.5782772633422316</v>
       </c>
       <c r="H17" t="n">
-        <v>0.2427927373398645</v>
+        <v>0.5797053311861768</v>
       </c>
       <c r="I17" t="n">
-        <v>0.2636546328138152</v>
+        <v>0.583009934301929</v>
       </c>
       <c r="J17" t="n">
-        <v>0.2897748490341038</v>
+        <v>0.6358928536473442</v>
       </c>
       <c r="K17" t="n">
-        <v>0.7478218636558492</v>
+        <v>0.591360892806673</v>
       </c>
       <c r="L17" t="n">
-        <v>0.249656579786262</v>
+        <v>0.6261033257984842</v>
       </c>
       <c r="M17" t="n">
-        <v>0.2504249277958301</v>
+        <v>0.5719116145016903</v>
       </c>
       <c r="N17" t="n">
-        <v>0.3565567727022813</v>
-      </c>
-      <c r="O17" t="n">
-        <v>0.2508553772214462</v>
+        <v>0.7992587313318554</v>
       </c>
     </row>
     <row r="18">
@@ -1381,34 +1328,31 @@
         <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.6640387420841678</v>
+        <v>0.6362982091857153</v>
       </c>
       <c r="G18" t="n">
-        <v>0.1914774984736885</v>
+        <v>0.5937815796285062</v>
       </c>
       <c r="H18" t="n">
-        <v>0.2000190373909477</v>
+        <v>0.6374169392014292</v>
       </c>
       <c r="I18" t="n">
-        <v>0.2688765158883483</v>
+        <v>0.6199883168474976</v>
       </c>
       <c r="J18" t="n">
-        <v>0.2682123033864766</v>
+        <v>0.6518736698166593</v>
       </c>
       <c r="K18" t="n">
-        <v>0.7037996867421685</v>
+        <v>0.5873766550716394</v>
       </c>
       <c r="L18" t="n">
-        <v>0.3501809421973322</v>
+        <v>0.6170725665584681</v>
       </c>
       <c r="M18" t="n">
-        <v>0.3114347773329301</v>
+        <v>0.633822776132321</v>
       </c>
       <c r="N18" t="n">
-        <v>0.1522845121567541</v>
-      </c>
-      <c r="O18" t="n">
-        <v>0.2349082125301026</v>
+        <v>0.8422107146169114</v>
       </c>
     </row>
     <row r="19">
@@ -1434,34 +1378,31 @@
         <v>1</v>
       </c>
       <c r="F19" t="n">
-        <v>-1.107400879733716</v>
+        <v>0.6806667755294935</v>
       </c>
       <c r="G19" t="n">
-        <v>0.347339177607937</v>
+        <v>0.7627773915002621</v>
       </c>
       <c r="H19" t="n">
-        <v>0.6492923955702398</v>
+        <v>0.7392070170497353</v>
       </c>
       <c r="I19" t="n">
-        <v>0.4181706787803032</v>
+        <v>0.6965323769896112</v>
       </c>
       <c r="J19" t="n">
-        <v>0.3914062694776969</v>
+        <v>0.7893830486487188</v>
       </c>
       <c r="K19" t="n">
-        <v>0.6588107456362138</v>
+        <v>0.6841546852991728</v>
       </c>
       <c r="L19" t="n">
-        <v>0.3287397902889628</v>
+        <v>0.8882132694836258</v>
       </c>
       <c r="M19" t="n">
-        <v>0.5303400442387239</v>
+        <v>0.670524649442804</v>
       </c>
       <c r="N19" t="n">
-        <v>0.8621662154782719</v>
-      </c>
-      <c r="O19" t="n">
-        <v>0.3521912712262327</v>
+        <v>0.8307266751065397</v>
       </c>
     </row>
     <row r="20">
@@ -1487,34 +1428,31 @@
         <v>1</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.3227047909551708</v>
+        <v>0.7341048996987063</v>
       </c>
       <c r="G20" t="n">
-        <v>0.2094056339755848</v>
+        <v>0.6418208799089163</v>
       </c>
       <c r="H20" t="n">
-        <v>0.3273011022142788</v>
+        <v>0.8518809067397505</v>
       </c>
       <c r="I20" t="n">
-        <v>0.2354635038536856</v>
+        <v>0.7709354435592145</v>
       </c>
       <c r="J20" t="n">
-        <v>0.2766604675248611</v>
+        <v>0.8853537884206309</v>
       </c>
       <c r="K20" t="n">
-        <v>0.7430843995336209</v>
+        <v>0.7027551762605483</v>
       </c>
       <c r="L20" t="n">
-        <v>0.2633574399511397</v>
+        <v>0.7938226937166013</v>
       </c>
       <c r="M20" t="n">
-        <v>0.2518973143680697</v>
+        <v>0.70355144149167</v>
       </c>
       <c r="N20" t="n">
-        <v>0.409735489923611</v>
-      </c>
-      <c r="O20" t="n">
-        <v>0.2784748908302692</v>
+        <v>0.8551609176166074</v>
       </c>
     </row>
     <row r="21">
@@ -1540,34 +1478,31 @@
         <v>1</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.09636687889850903</v>
+        <v>0.6144618063131096</v>
       </c>
       <c r="G21" t="n">
-        <v>0.2803610324661884</v>
+        <v>0.6086739195700983</v>
       </c>
       <c r="H21" t="n">
-        <v>0.3937130849667385</v>
+        <v>0.7372064946676444</v>
       </c>
       <c r="I21" t="n">
-        <v>0.2862780413145777</v>
+        <v>0.6096867904141217</v>
       </c>
       <c r="J21" t="n">
-        <v>0.3010800891458826</v>
+        <v>0.6440304757997999</v>
       </c>
       <c r="K21" t="n">
-        <v>0.769638303072412</v>
+        <v>0.6551931917204481</v>
       </c>
       <c r="L21" t="n">
-        <v>0.3182117492692488</v>
+        <v>0.6984921468127152</v>
       </c>
       <c r="M21" t="n">
-        <v>0.2629558359801659</v>
+        <v>0.6416968656370493</v>
       </c>
       <c r="N21" t="n">
-        <v>0.3683983310593923</v>
-      </c>
-      <c r="O21" t="n">
-        <v>0.2579204342093958</v>
+        <v>0.8375956833985226</v>
       </c>
     </row>
     <row r="22">
@@ -1593,34 +1528,31 @@
         <v>1</v>
       </c>
       <c r="F22" t="n">
-        <v>0.298650936879099</v>
+        <v>0.5649426802959302</v>
       </c>
       <c r="G22" t="n">
-        <v>0.5121723496042556</v>
+        <v>0.5611258797105646</v>
       </c>
       <c r="H22" t="n">
-        <v>0.3590113314252176</v>
+        <v>0.5620057222528267</v>
       </c>
       <c r="I22" t="n">
-        <v>0.4356322078536043</v>
+        <v>0.5675120687147992</v>
       </c>
       <c r="J22" t="n">
-        <v>0.4601860729658694</v>
+        <v>0.6137617611741494</v>
       </c>
       <c r="K22" t="n">
-        <v>0.8159760480750113</v>
+        <v>0.7304820535140963</v>
       </c>
       <c r="L22" t="n">
-        <v>0.3728421429240272</v>
+        <v>0.6191284375737034</v>
       </c>
       <c r="M22" t="n">
-        <v>0.3591514826768604</v>
+        <v>0.5644383792241516</v>
       </c>
       <c r="N22" t="n">
-        <v>0.3509718394356887</v>
-      </c>
-      <c r="O22" t="n">
-        <v>0.4130297764902056</v>
+        <v>0.7974167652382866</v>
       </c>
     </row>
     <row r="23">
@@ -1646,34 +1578,31 @@
         <v>1</v>
       </c>
       <c r="F23" t="n">
-        <v>0.1912005181776173</v>
+        <v>0.7159236837559406</v>
       </c>
       <c r="G23" t="n">
-        <v>0.4364556868657948</v>
+        <v>0.6606679631802898</v>
       </c>
       <c r="H23" t="n">
-        <v>0.3093084264703347</v>
+        <v>0.6829178424798934</v>
       </c>
       <c r="I23" t="n">
-        <v>0.3493979849081216</v>
+        <v>0.7432119238151129</v>
       </c>
       <c r="J23" t="n">
-        <v>0.3934539751368294</v>
+        <v>0.8456817478080344</v>
       </c>
       <c r="K23" t="n">
-        <v>0.8037184033040029</v>
+        <v>0.7150136676326554</v>
       </c>
       <c r="L23" t="n">
-        <v>0.4040927187333575</v>
+        <v>0.8453911053076802</v>
       </c>
       <c r="M23" t="n">
-        <v>0.3251386563633973</v>
+        <v>0.6777267054156471</v>
       </c>
       <c r="N23" t="n">
-        <v>0.3428268670094803</v>
-      </c>
-      <c r="O23" t="n">
-        <v>0.3787537548649644</v>
+        <v>0.8413271756719426</v>
       </c>
     </row>
     <row r="24">
@@ -1699,34 +1628,31 @@
         <v>1</v>
       </c>
       <c r="F24" t="n">
-        <v>-1.451663169588896</v>
+        <v>0.6322637076424887</v>
       </c>
       <c r="G24" t="n">
-        <v>0.5717124853322739</v>
+        <v>0.6145203577433802</v>
       </c>
       <c r="H24" t="n">
-        <v>0.7299061371819893</v>
+        <v>0.6536669564603145</v>
       </c>
       <c r="I24" t="n">
-        <v>0.6146609287772477</v>
+        <v>0.6204729134081688</v>
       </c>
       <c r="J24" t="n">
-        <v>0.6155464648401392</v>
+        <v>0.6581745084808737</v>
       </c>
       <c r="K24" t="n">
-        <v>0.6400911217032833</v>
+        <v>0.9068167041316114</v>
       </c>
       <c r="L24" t="n">
-        <v>0.6522510810891509</v>
+        <v>0.7748665695067382</v>
       </c>
       <c r="M24" t="n">
-        <v>0.7399460337843894</v>
+        <v>0.6352118876799946</v>
       </c>
       <c r="N24" t="n">
-        <v>1.048797355368231</v>
-      </c>
-      <c r="O24" t="n">
-        <v>0.5675910868027001</v>
+        <v>0.8341246528954248</v>
       </c>
     </row>
     <row r="25">
@@ -1752,34 +1678,31 @@
         <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.1203686219198782</v>
+        <v>0.5889810475808932</v>
       </c>
       <c r="G25" t="n">
-        <v>0.2665965921611493</v>
+        <v>0.5867506107788001</v>
       </c>
       <c r="H25" t="n">
-        <v>0.3881895738973692</v>
+        <v>0.5762842947476078</v>
       </c>
       <c r="I25" t="n">
-        <v>0.2853736705985076</v>
+        <v>0.5803818083840081</v>
       </c>
       <c r="J25" t="n">
-        <v>0.317474040658008</v>
+        <v>0.6135909504333112</v>
       </c>
       <c r="K25" t="n">
-        <v>0.7676949679739734</v>
+        <v>0.6199004693791328</v>
       </c>
       <c r="L25" t="n">
-        <v>0.2981247450723863</v>
+        <v>0.6003965938727117</v>
       </c>
       <c r="M25" t="n">
-        <v>0.260684823520987</v>
+        <v>0.5858136934860649</v>
       </c>
       <c r="N25" t="n">
-        <v>0.1597775121464154</v>
-      </c>
-      <c r="O25" t="n">
-        <v>0.3574792898582413</v>
+        <v>0.8199943522940039</v>
       </c>
     </row>
   </sheetData>

</xml_diff>